<commit_message>
10th commit : code optimize
</commit_message>
<xml_diff>
--- a/manual.xlsx
+++ b/manual.xlsx
@@ -8,42 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijung\PycharmProjects\Load_Spectrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8DCAD6-02EF-4415-8EA8-96A2A8D91D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A1EADB-75BF-4911-BC59-D83F0F791CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D960881-CEBA-4B13-9696-05E483397A48}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6D960881-CEBA-4B13-9696-05E483397A48}"/>
   </bookViews>
   <sheets>
-    <sheet name="Interface" sheetId="1" r:id="rId1"/>
-    <sheet name="파일 송수신" sheetId="4" r:id="rId2"/>
-    <sheet name="설정방법" sheetId="2" r:id="rId3"/>
-    <sheet name="예시" sheetId="3" r:id="rId4"/>
+    <sheet name="간편사용법" sheetId="5" r:id="rId1"/>
+    <sheet name="Interface" sheetId="1" r:id="rId2"/>
+    <sheet name="파일 송수신" sheetId="4" r:id="rId3"/>
+    <sheet name="설정" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
   <si>
     <t>&lt;초기화면&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;경로 제어 예시&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -150,10 +137,6 @@
   </si>
   <si>
     <t>Line - EQP - Drive를 선택하여 설비로 FTP 접속</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FileZilla 설정 포함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -452,15 +435,229 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>내 PC에서 경로를 제어할 Drive 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>- 기본적으로 C, D, E 3가지가 있으며 PC 내 Drive가 없는 Drive 선택하면 Local Path에 '파일없음'이라고 표시됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>원하는 경로 추가하기</t>
+    <t>내 PC에서 경로를 제어할 Path 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 등록된 Drive Path가 표시됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 제어하려는 Drive Path를 클릭하면 하단에 파일 리스트 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 'Drive 등록' Push 버튼 눌러서 상단 Naming Rule에 맞게 사용자 정의 Path 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- ex) C:\0.path_test\Lot Raw Data 를 Raw Data라는 Name으로 Path에 추가할 때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 실제 폴더 만들고 경로 복사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Drive 등록 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4. 프로그램 종료 후 실행 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>※ 반드시 경로 앞에 #으로 구분지어야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. PathName # (복사한 경로) 추가 &amp; 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제어하고 있는 Local 경로를 나타냄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local Path 영역으로 현재 제어중인 경로의 파일 리스트를 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 폴더 더블클릭하면 해당 폴더로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 파일 더블클릭하면 파일 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local Path 제어 부가 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 현재 Path 기준 뒤로가기, 앞으로가기, 새폴더, 삭제 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 뒤로가기의 경우 최대 Drive 경로까지 접근 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- ex) Drive에서 최초로 접근한 Path가 Drive 하위 경로일 때 뒤로가기 누르면 C:로 이동함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;경로 제어 화면&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11~18호기 Lot 옮기는 파일 송수신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">- FTP를 이용하여 파일을 송수신하므로 접속하려는 설비 PC에 FTP 설정 필요 : FileZilla Server 설정 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a. FileZilla FTP 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b. Listwidget 지원 Icon</t>
+  </si>
+  <si>
+    <t>b. Listwidget 지원 Icon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 설비 오른쪽 아래 트레이에서 FileZilla 아이콘 더블클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Edit → User 또는 아래 사람 그림 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Add → 계정명 입력 후 OK → Password 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Shared folders → Users 선택 → Add → Path 선택 → Files, Directories 권한 All Check </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LS_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LS_D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LS_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>→ FileZilla Server에 해당 계정 설정되어 있어야 프로그램 사용 가능</t>
+  </si>
+  <si>
+    <t>0. 파이썬 프로그램에서 접속하고 있는 FTP ID / PW List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>※ 이하 FileZilla Server 설정 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type(확장자)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>txt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>py</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bmp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,12 +748,64 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -565,7 +814,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -598,6 +847,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1988,8 +2267,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4455459" y="4518212"/>
-          <a:ext cx="2070847" cy="2814916"/>
+          <a:off x="4444701" y="4455459"/>
+          <a:ext cx="2065469" cy="2777264"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2308,8 +2587,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="443754" y="9529482"/>
-          <a:ext cx="4782670" cy="1775012"/>
+          <a:off x="443754" y="9397701"/>
+          <a:ext cx="4770119" cy="1749911"/>
           <a:chOff x="443754" y="9529482"/>
           <a:chExt cx="4782670" cy="1775012"/>
         </a:xfrm>
@@ -5552,25 +5831,25 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>421342</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>98613</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>204094</xdr:colOff>
-      <xdr:row>181</xdr:row>
-      <xdr:rowOff>35859</xdr:rowOff>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>20039</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>91829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>294012</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="132" name="그림 131">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{830ECB73-6D36-4D9C-A6C1-EAB2EBC26B68}"/>
+        <xdr:cNvPr id="133" name="그림 132">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29CC49CA-85E8-48B2-B9A4-A56C55AFED85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5579,14 +5858,2783 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:srcRect l="65496" t="3852" r="24231" b="74500"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="65636" t="4814" r="1" b="74771"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="421342" y="38870966"/>
-          <a:ext cx="1127458" cy="1730187"/>
+          <a:off x="4043399" y="39647249"/>
+          <a:ext cx="2956213" cy="1264531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>38502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>455404</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="135" name="직사각형 134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA488ED-1BC1-482B-8B47-401C6902AB4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5661660" y="39814902"/>
+          <a:ext cx="828784" cy="258678"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>649877</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>85996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>176348</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="138" name="그림 137">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8364AB7D-4459-4ED5-BE60-624480A46331}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:srcRect l="20065" t="8654" r="61003" b="66657"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1320437" y="39641416"/>
+          <a:ext cx="2253343" cy="1637212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>379373</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>183282</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="144" name="직사각형 143">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA85CC4B-7688-4D51-A14A-DB8F5D75B154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1720493" y="40843602"/>
+          <a:ext cx="1571347" cy="296778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>84725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>161364</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="145" name="그림 144">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08DD18A3-B4F5-4D29-A53E-3E60D8FB2EBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:srcRect r="45172" b="56338"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7386469" y="40425901"/>
+          <a:ext cx="3087445" cy="1645463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22796</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>95409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>388555</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>8324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="146" name="그림 145">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{291298D4-ABCC-4A9A-9122-85D0A29AD6E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:srcRect l="59472" t="7602" r="17864" b="76049"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10751756" y="39650829"/>
+          <a:ext cx="3047999" cy="1238795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>2642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>340658</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="147" name="직사각형 146">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5714EAC0-BBC0-4578-93D5-E29561E2707E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7325509" y="41688524"/>
+          <a:ext cx="3100443" cy="266299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>146573</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>128148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>172123</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="148" name="직사각형 147">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037B6A07-07D2-4840-8705-A2331963D4EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10875533" y="40567488"/>
+          <a:ext cx="2707790" cy="272126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>398930</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>8966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>605118</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>215154</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="149" name="타원 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B226E919-98FA-43B2-962F-DB83B48925A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="398930" y="37796546"/>
+          <a:ext cx="206188" cy="206188"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="0000FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1"/>
+            <a:t>2</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68579</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>7621</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>215901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="150" name="그림 149">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26F73B6-7375-4FB7-B45B-CAA25B709786}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="65851" t="6975" r="1523" b="69280"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739139" y="42214801"/>
+          <a:ext cx="2506981" cy="1313180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>398930</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>8966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>605118</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>215154</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="152" name="타원 151">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021CFA39-59DF-4B92-B0A1-E922ED65C15C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="398930" y="41774186"/>
+          <a:ext cx="206188" cy="206188"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="0000FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1"/>
+            <a:t>3</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>634124</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>87118</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>35753</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="153" name="그림 152">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B977A348-98DB-4F83-9E6C-B8EDD0C733A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="634124" y="44683680"/>
+          <a:ext cx="2805794" cy="2420813"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>65284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>363351</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>1709</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="154" name="그림 153">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0B246DD-C2B4-494A-BAFF-8FF9BF80ADCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3832860" y="45808144"/>
+          <a:ext cx="3236091" cy="1262305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>199467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>199468</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="155" name="직선 화살표 연결선 154">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{311C2CE0-755C-4074-9874-DD6E72D28126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3063240" y="46605267"/>
+          <a:ext cx="685800" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>398930</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>8966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>605118</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>215154</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="158" name="타원 157">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{294E7710-B610-4CA3-884F-9EE9C5D31193}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="398930" y="43983986"/>
+          <a:ext cx="206188" cy="206188"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="0000FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1"/>
+            <a:t>4</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>213361</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>217</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="159" name="그림 158">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97976049-6902-4427-AC05-18E0429176D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:srcRect t="24407" r="4164" b="52654"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5074921" y="47724061"/>
+          <a:ext cx="3101339" cy="289559"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>580813</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142371</xdr:colOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>121534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="160" name="그림 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7C4438-2E35-4AEB-A55C-681726BF55FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1251373" y="48493680"/>
+          <a:ext cx="2914358" cy="2232274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>98668</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>92834</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>72001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="161" name="그림 160">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DEAB6B0-97F2-4284-B37D-65B579152F94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305300" y="48493288"/>
+          <a:ext cx="3163694" cy="2404113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>67737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>542247</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="162" name="그림 161">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8914BD3B-C36C-4717-83AF-5EAA3354E1D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7612380" y="48462357"/>
+          <a:ext cx="2988267" cy="2446864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>54689</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="163" name="직선 화살표 연결선 162">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EB5F0D-0A03-4A08-B240-273AABBB1FBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1661160" y="50116740"/>
+          <a:ext cx="2773680" cy="100409"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>662941</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>335281</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="164" name="직사각형 163">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B522C23-E4AA-4F0E-B862-723A5E255429}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333501" y="50124360"/>
+          <a:ext cx="342900" cy="243840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>411481</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83821</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="167" name="직사각형 166">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD011C19-B360-457E-9016-F250B6ABC67E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4434841" y="50208180"/>
+          <a:ext cx="342900" cy="243840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>123270</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="168" name="직선 화살표 연결선 167">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7480208-6F5D-4C7B-BFED-A0E7F38AF949}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4777740" y="50048160"/>
+          <a:ext cx="2918460" cy="237570"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>621194</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28244</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>5851</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D74495C4-8F34-4877-9715-8E921A2738A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2277716" y="5826070"/>
+          <a:ext cx="3851415" cy="1841194"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60319</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>6164</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>384729</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9FC4E3B-1C43-4EC5-A903-C2DF0DF456BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="24013" t="19261" r="64313" b="67667"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6529036" y="1248555"/>
+          <a:ext cx="1699323" cy="1057738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>187778</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>441877</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>173169</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0249DEA5-6F66-41F1-9675-A0A776045608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect l="81533" t="84530" r="5053"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2530928" y="1285877"/>
+          <a:ext cx="1841047" cy="1192342"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>559905</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>23072</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B00090D-E7DC-491D-97B7-5773A9BC2072}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect l="23857" t="19619" r="66915" b="72406"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8403535" y="1283803"/>
+          <a:ext cx="1692966" cy="809921"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>182218</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>496957</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165652</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="직사각형 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{852CDD30-9887-4FA8-9367-D620279C2AFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9400761" y="1681370"/>
+          <a:ext cx="314739" cy="347869"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107047</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314740</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>170642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68676FE2-188F-4220-B6D8-4BD606DD9679}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2352261" y="3213025"/>
+          <a:ext cx="3743740" cy="1927182"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>654325</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>149089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>422413</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>124240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="직사각형 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BBA8EDD-6AAD-482F-ABDC-242AF7A30AD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5060673" y="4497459"/>
+          <a:ext cx="455544" cy="182216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>405846</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>182221</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>612912</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>173935</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="직사각형 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C15842E5-80F7-4B37-8746-3BB8135B9E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3437281" y="4323525"/>
+          <a:ext cx="1581979" cy="198780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438979</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>49695</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>579783</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>141983</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52E60B56-443E-4601-BA00-574249B77FE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6220240" y="3155673"/>
+          <a:ext cx="4265543" cy="1955875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>662607</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="직사각형 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{446E3ED7-F0FF-4D6B-B450-576DCF1C1901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7818781" y="3652633"/>
+          <a:ext cx="1093306" cy="157367"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>405849</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>163679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>306457</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>198832</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="그림 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C293ECBF-EE6B-446E-8375-3900E5E6A181}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6874566" y="5754440"/>
+          <a:ext cx="4025347" cy="3141131"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>115954</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>41415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>629479</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>173934</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="직사각형 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A8B0B3-A658-46D3-8503-EAA8C2DB9272}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2459932" y="6253372"/>
+          <a:ext cx="513525" cy="132519"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>115954</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>99393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>530088</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="직사각형 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFC9CA9A-9F15-4A38-A989-BA9C71C3A660}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3147389" y="7346676"/>
+          <a:ext cx="414134" cy="132520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>24845</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>82828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>298174</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="직사각형 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45F3DF8A-1925-4B18-A5D9-94E0CF8E34C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5118649" y="6501850"/>
+          <a:ext cx="273329" cy="124237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>339586</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>188306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>636163</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>59529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="그림 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1F50EB-A5BB-4D47-BF4A-A6D4D4D2C57F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11620499" y="5572002"/>
+          <a:ext cx="4421316" cy="2977202"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>455540</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>115959</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>530087</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>74542</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="직사각형 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E151289A-174A-45CE-B077-6472A4FDB03B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7611714" y="8191502"/>
+          <a:ext cx="762003" cy="165649"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>538370</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>190502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438978</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="직사각형 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD409A9B-C708-4491-BCA8-4C1CE4ED8BBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="8680176"/>
+          <a:ext cx="588065" cy="223628"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>670891</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>91110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>596348</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>173934</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="직사각형 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C73D7F-9F1D-412A-8D40-60E9708300F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14014174" y="5888936"/>
+          <a:ext cx="612913" cy="1325215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>372717</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>496956</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>198783</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="직사각형 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D33079D-6B9A-444F-83B8-8F9E729F39DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11653630" y="8083827"/>
+          <a:ext cx="811696" cy="190499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>405848</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>289892</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="직선 화살표 연결선 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D71C24AE-6CEE-4823-A8CF-E62E2B618C72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6187109" y="6568109"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>306457</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="직선 화살표 연결선 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5C0689B-CD9D-4BD8-B8B0-2276C277A6B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10899914" y="6568109"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>206191</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>17931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>412379</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="그림 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{465EA760-2D23-409A-96BC-CD1CF1501FF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3433485" y="12568519"/>
+          <a:ext cx="206188" cy="206188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>206190</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>416300</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="그림 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1FEB5FD-8A05-4DD9-BF8B-C87B088158F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3433484" y="12819530"/>
+          <a:ext cx="210110" cy="179294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215153</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>403411</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>215152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="그림 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B218E30-A3F0-4C74-AE95-1E294B9BDA31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3442447" y="13025718"/>
+          <a:ext cx="188258" cy="188258"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215155</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>35861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>385483</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>206189</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="그림 33" descr="텍스트, 명함, 벡터그래픽이(가) 표시된 사진&#10;&#10;자동 생성된 설명">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53B4C83-00B0-44BC-AC65-298379A75ED2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3442449" y="13258802"/>
+          <a:ext cx="170328" cy="170328"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>206189</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>376519</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>197224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="그림 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C344B4-FC6A-434E-B2DC-E78642539F9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3433483" y="13473953"/>
+          <a:ext cx="170330" cy="170330"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215153</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>35860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361092</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>215154</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="그림 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D41DDE0-2F9B-40F7-B13B-B2BB55F0D0C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3442447" y="13707036"/>
+          <a:ext cx="145939" cy="179294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>197227</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>215153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>385487</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>179296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="그림 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131BAABD-E1D3-4E38-A9F8-967AB5566D68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3424521" y="14334565"/>
+          <a:ext cx="188260" cy="188260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5894,53 +8942,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F290DE-6907-4C44-B4E4-F5B7FE0B14FB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9921FC81-D07D-40FD-BC52-B33AF2A57A53}">
-  <dimension ref="A1:R174"/>
+  <dimension ref="A1:R219"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
@@ -5948,310 +9011,388 @@
         <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
         <v>10</v>
       </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
       <c r="M37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.4">
       <c r="M38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.4">
       <c r="I44" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.4">
       <c r="I45" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.4">
       <c r="I46" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.4">
       <c r="I47" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B54" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B55" s="7"/>
       <c r="C55" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C67" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R67" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C68" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R68" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="R68" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C69" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R69" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C70" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B73" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C74" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C75" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C76" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C77" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C78" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C79" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B82" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B91" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C91" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q91" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.4">
       <c r="C92" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q92" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="2:17" x14ac:dyDescent="0.4">
       <c r="C93" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="94" spans="2:17" x14ac:dyDescent="0.4">
       <c r="C94" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B111" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C111" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C112" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C113" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C114" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B120" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C120" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.4">
       <c r="K122" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.4">
       <c r="K123" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="124" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C124" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E124" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.4">
       <c r="K125" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.4">
       <c r="K126" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.4">
       <c r="H128" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="145" spans="8:16" x14ac:dyDescent="0.4">
       <c r="H145" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P145" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="146" spans="8:16" x14ac:dyDescent="0.4">
       <c r="H146" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P146" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="147" spans="8:16" x14ac:dyDescent="0.4">
       <c r="H147" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P147" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="148" spans="8:16" x14ac:dyDescent="0.4">
       <c r="P148" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B172" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C172" t="s">
         <v>75</v>
       </c>
-      <c r="C172" t="s">
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C173" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C174" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="C173" s="2" t="s">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C175" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="D174" t="s">
+    <row r="177" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="C177" s="10" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="179" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="C179" t="s">
+        <v>80</v>
+      </c>
+      <c r="G179" t="s">
+        <v>81</v>
+      </c>
+      <c r="L179" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q179" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="180" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="L180" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="190" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B190" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C190" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B200" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C200" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C201" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C202" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B216" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C216" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C217" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C218" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C219" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -6262,34 +9403,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0BC8B5-E5AA-4C5E-8E4A-1C0211A732CA}">
-  <dimension ref="A1"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF67905-9AC7-4269-AA98-30D78D3444FF}">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>12</v>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -6299,16 +9425,203 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5CE6A8-AA1A-4A67-9CD4-872C2AFAADAD}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF67905-9AC7-4269-AA98-30D78D3444FF}">
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.69921875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C5" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C6" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C7" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C8" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C9" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C10" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C12" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C55" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C56" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C57" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="17"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C58" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="17"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C59" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="17"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C60" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="17"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C61" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="17"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C62" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62" s="17"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C63" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C64" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="19"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C65" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="19"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C66" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D66" s="19"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C67" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D63:D67"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>